<commit_message>
The other half of the doodles...
</commit_message>
<xml_diff>
--- a/alistair/doodles.xlsx
+++ b/alistair/doodles.xlsx
@@ -1,33 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ammoffat/tex/16/ymt16airs/alistair/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25317"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>rho</t>
   </si>
@@ -40,14 +36,24 @@
   <si>
     <t>1+floor()</t>
   </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>RBP</t>
+  </si>
+  <si>
+    <t>smoothed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="0.00000"/>
-    <numFmt numFmtId="168" formatCode="0.000000"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -58,12 +64,48 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -78,11 +120,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -140,7 +189,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -175,7 +224,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -352,7 +401,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -363,12 +412,12 @@
   <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -383,7 +432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>1</v>
       </c>
@@ -391,24 +440,24 @@
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <f>B4-1</f>
+        <f t="shared" ref="C3:C12" si="0">B4-1</f>
         <v>2</v>
       </c>
       <c r="H3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4">
         <f>A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <f>CEILING(B3*B$1,1)</f>
+        <f t="shared" ref="B4:B12" si="1">CEILING(B3*B$1,1)</f>
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <f>B5-1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="K4" t="s">
@@ -418,17 +467,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5">
-        <f t="shared" ref="A5:A21" si="0">A4+1</f>
+        <f t="shared" ref="A5:A21" si="2">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <f>CEILING(B4*B$1,1)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="C5" s="1">
-        <f>B6-1</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="H5">
@@ -438,25 +487,25 @@
         <v>11</v>
       </c>
       <c r="K5" s="2">
-        <f t="shared" ref="K5:K18" si="1">1/(H5-1)</f>
+        <f t="shared" ref="K5:K15" si="3">1/(H5-1)</f>
         <v>9.9999999999999911</v>
       </c>
       <c r="L5" s="2">
-        <f>1+FLOOR(K5+0.000001,1)</f>
+        <f t="shared" ref="L5:L18" si="4">1+FLOOR(K5+0.000001,1)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <f>CEILING(B5*B$1,1)</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="C6" s="1">
-        <f>B7-1</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="H6">
@@ -466,25 +515,25 @@
         <v>6</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.0000000000000009</v>
       </c>
       <c r="L6" s="2">
-        <f>1+FLOOR(K6+0.000001,1)</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <f>CEILING(B6*B$1,1)</f>
+        <f t="shared" si="1"/>
         <v>81</v>
       </c>
       <c r="C7" s="1">
-        <f>B8-1</f>
+        <f t="shared" si="0"/>
         <v>242</v>
       </c>
       <c r="H7">
@@ -494,25 +543,25 @@
         <v>5</v>
       </c>
       <c r="K7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="L7" s="2">
-        <f>1+FLOOR(K7+0.000001,1)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <f>CEILING(B7*B$1,1)</f>
+        <f t="shared" si="1"/>
         <v>243</v>
       </c>
       <c r="C8" s="1">
-        <f>B9-1</f>
+        <f t="shared" si="0"/>
         <v>728</v>
       </c>
       <c r="H8">
@@ -522,25 +571,25 @@
         <v>4</v>
       </c>
       <c r="K8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.333333333333333</v>
       </c>
       <c r="L8" s="2">
-        <f>1+FLOOR(K8+0.000001,1)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="A9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <f>CEILING(B8*B$1,1)</f>
+        <f t="shared" si="1"/>
         <v>729</v>
       </c>
       <c r="C9" s="1">
-        <f>B10-1</f>
+        <f t="shared" si="0"/>
         <v>2186</v>
       </c>
       <c r="H9">
@@ -550,25 +599,25 @@
         <v>3</v>
       </c>
       <c r="K9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.8571428571428563</v>
       </c>
       <c r="L9" s="2">
-        <f>1+FLOOR(K9+0.000001,1)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <f>CEILING(B9*B$1,1)</f>
+        <f t="shared" si="1"/>
         <v>2187</v>
       </c>
       <c r="C10" s="1">
-        <f>B11-1</f>
+        <f t="shared" si="0"/>
         <v>6560</v>
       </c>
       <c r="H10">
@@ -578,25 +627,25 @@
         <v>3</v>
       </c>
       <c r="K10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.5000000000000004</v>
       </c>
       <c r="L10" s="2">
-        <f>1+FLOOR(K10+0.000001,1)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="A11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="B11" s="1">
-        <f>CEILING(B10*B$1,1)</f>
+        <f t="shared" si="1"/>
         <v>6561</v>
       </c>
       <c r="C11" s="1">
-        <f>B12-1</f>
+        <f t="shared" si="0"/>
         <v>19682</v>
       </c>
       <c r="H11">
@@ -606,25 +655,25 @@
         <v>3</v>
       </c>
       <c r="K11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.2222222222222223</v>
       </c>
       <c r="L11" s="2">
-        <f>1+FLOOR(K11+0.000001,1)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="A12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <f>CEILING(B11*B$1,1)</f>
+        <f t="shared" si="1"/>
         <v>19683</v>
       </c>
       <c r="C12" s="1">
-        <f>B13-1</f>
+        <f t="shared" si="0"/>
         <v>59048</v>
       </c>
       <c r="H12">
@@ -634,25 +683,25 @@
         <v>3</v>
       </c>
       <c r="K12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L12" s="2">
-        <f>1+FLOOR(K12+0.000001,1)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="A13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" ref="B13:B22" si="2">CEILING(B12*B$1,1)</f>
+        <f t="shared" ref="B13:B22" si="5">CEILING(B12*B$1,1)</f>
         <v>59049</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" ref="C13:C22" si="3">B14-1</f>
+        <f t="shared" ref="C13:C22" si="6">B14-1</f>
         <v>177146</v>
       </c>
       <c r="H13">
@@ -662,25 +711,25 @@
         <v>2</v>
       </c>
       <c r="K13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.6666666666666665</v>
       </c>
       <c r="L13" s="2">
-        <f>1+FLOOR(K13+0.000001,1)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="A14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>177147</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>531440</v>
       </c>
       <c r="H14">
@@ -690,25 +739,25 @@
         <v>2</v>
       </c>
       <c r="K14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.4285714285714286</v>
       </c>
       <c r="L14" s="2">
-        <f>1+FLOOR(K14+0.000001,1)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="A15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>531441</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1594322</v>
       </c>
       <c r="H15">
@@ -718,25 +767,25 @@
         <v>2</v>
       </c>
       <c r="K15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.1111111111111112</v>
       </c>
       <c r="L15" s="2">
-        <f>1+FLOOR(K15+0.000001,1)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="A16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="B16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1594323</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4782968</v>
       </c>
       <c r="H16">
@@ -750,21 +799,21 @@
         <v>1</v>
       </c>
       <c r="L16" s="2">
-        <f>1+FLOOR(K16+0.000001,1)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12">
       <c r="A17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4782969</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>14348906</v>
       </c>
       <c r="H17">
@@ -774,25 +823,25 @@
         <v>1</v>
       </c>
       <c r="K17" s="2">
-        <f t="shared" ref="K17:K18" si="4">1/(H17-1)</f>
+        <f t="shared" ref="K17:K18" si="7">1/(H17-1)</f>
         <v>0.90909090909090906</v>
       </c>
       <c r="L17" s="2">
-        <f>1+FLOOR(K17+0.000001,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>14348907</v>
       </c>
       <c r="C18" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>43046720</v>
       </c>
       <c r="H18">
@@ -802,67 +851,67 @@
         <v>1</v>
       </c>
       <c r="K18" s="2">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="L18" s="2">
         <f t="shared" si="4"/>
-        <v>0.5</v>
-      </c>
-      <c r="L18" s="2">
-        <f>1+FLOOR(K18+0.000001,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>43046721</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>129140162</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12">
       <c r="A20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>129140163</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>387420488</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="A21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="B21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>387420489</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1162261466</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12">
       <c r="B22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1162261467</v>
       </c>
       <c r="C22" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="5:6">
       <c r="E33">
         <v>0.5</v>
       </c>
@@ -870,7 +919,7 @@
         <v>0.50000100000000003</v>
       </c>
     </row>
-    <row r="34" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="5:6">
       <c r="E34">
         <v>0.6</v>
       </c>
@@ -878,7 +927,7 @@
         <v>0.59999899999999995</v>
       </c>
     </row>
-    <row r="35" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="5:6">
       <c r="E35">
         <v>0.5</v>
       </c>
@@ -886,7 +935,7 @@
         <v>0.49999900000000003</v>
       </c>
     </row>
-    <row r="36" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="5:6">
       <c r="E36">
         <v>0.4</v>
       </c>
@@ -894,7 +943,7 @@
         <v>0.400001</v>
       </c>
     </row>
-    <row r="37" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="5:6">
       <c r="E37">
         <v>0.5</v>
       </c>
@@ -902,7 +951,7 @@
         <v>0.50000100000000003</v>
       </c>
     </row>
-    <row r="38" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="5:6">
       <c r="E38">
         <v>0.6</v>
       </c>
@@ -910,7 +959,7 @@
         <v>0.59999899999999995</v>
       </c>
     </row>
-    <row r="39" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="5:6">
       <c r="E39">
         <v>0.3</v>
       </c>
@@ -918,7 +967,7 @@
         <v>0.29999900000000002</v>
       </c>
     </row>
-    <row r="40" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="5:6">
       <c r="E40">
         <v>0.4</v>
       </c>
@@ -926,7 +975,7 @@
         <v>0.39999899999999999</v>
       </c>
     </row>
-    <row r="41" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="5:6">
       <c r="E41">
         <v>0.4</v>
       </c>
@@ -934,7 +983,7 @@
         <v>0.400001</v>
       </c>
     </row>
-    <row r="42" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="5:6">
       <c r="E42">
         <v>0.3</v>
       </c>
@@ -942,7 +991,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="45" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="5:6">
       <c r="F45">
         <f>TTEST(E33:E42,F33:F42,2,1)</f>
         <v>0.75773932912276754</v>
@@ -950,5 +999,729 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:L37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="9" max="9" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1">
+        <v>0.9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="4">
+        <f>ABS(G36-H36)</f>
+        <v>7.9511854302853291E-2</v>
+      </c>
+      <c r="J1">
+        <v>0.10159493</v>
+      </c>
+      <c r="K1">
+        <v>0.10358235</v>
+      </c>
+      <c r="L1">
+        <v>7.9970059999999996E-2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12">
+      <c r="J2">
+        <v>0.5</v>
+      </c>
+      <c r="K2">
+        <v>0.7</v>
+      </c>
+      <c r="L2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12">
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <f>(1-C1)</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="D3" s="3">
+        <f>SUM(C3)</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3*C3</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <f>D3*AVERAGE(F3:F3)</f>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12">
+      <c r="B4" s="6">
+        <f>B3+1</f>
+        <v>2</v>
+      </c>
+      <c r="C4" s="3">
+        <f>C3*C$1</f>
+        <v>8.9999999999999983E-2</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" ref="G4:G33" si="0">F4*C4</f>
+        <v>8.9999999999999983E-2</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12">
+      <c r="B5" s="6">
+        <f t="shared" ref="B5:B33" si="1">B4+1</f>
+        <v>3</v>
+      </c>
+      <c r="C5" s="3">
+        <f>C4*C$1</f>
+        <v>8.0999999999999989E-2</v>
+      </c>
+      <c r="D5" s="3">
+        <f>SUM(C4:C5)</f>
+        <v>0.17099999999999999</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <f>D5*AVERAGE(F4:F5)</f>
+        <v>8.5499999999999993E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12">
+      <c r="B6" s="7">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C6" s="3">
+        <f>C5*C$1</f>
+        <v>7.2899999999999993E-2</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="F6" s="8">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <f t="shared" si="0"/>
+        <v>7.2899999999999993E-2</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
+      <c r="B7" s="7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C7" s="3">
+        <f>C6*C$1</f>
+        <v>6.5610000000000002E-2</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="F7" s="8">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" si="0"/>
+        <v>6.5610000000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
+      <c r="B8" s="7">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C8" s="3">
+        <f>C7*C$1</f>
+        <v>5.9049000000000004E-2</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="F8" s="8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12">
+      <c r="B9" s="7">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C9" s="3">
+        <f>C8*C$1</f>
+        <v>5.3144100000000007E-2</v>
+      </c>
+      <c r="D9" s="3">
+        <f>SUM(C6:C9)</f>
+        <v>0.25070310000000001</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <f>D9*AVERAGE(F6:F9)</f>
+        <v>0.12535155000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12">
+      <c r="B10" s="9">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="C10" s="3">
+        <f>C9*C$1</f>
+        <v>4.7829690000000008E-2</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="F10" s="9">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" si="0"/>
+        <v>4.7829690000000008E-2</v>
+      </c>
+      <c r="J10">
+        <v>3</v>
+      </c>
+      <c r="K10">
+        <v>3</v>
+      </c>
+      <c r="L10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12">
+      <c r="B11" s="9">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="C11" s="3">
+        <f>C10*C$1</f>
+        <v>4.304672100000001E-2</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="F11" s="9">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" si="0"/>
+        <v>4.304672100000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12">
+      <c r="B12" s="9">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C12" s="3">
+        <f>C11*C$1</f>
+        <v>3.8742048900000013E-2</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="F12" s="9">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8742048900000013E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12">
+      <c r="B13" s="9">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="C13" s="3">
+        <f>C12*C$1</f>
+        <v>3.486784401000001E-2</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="F13" s="9">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" si="0"/>
+        <v>3.486784401000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12">
+      <c r="B14" s="9">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="C14" s="3">
+        <f>C13*C$1</f>
+        <v>3.1381059609000013E-2</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="F14" s="9">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12">
+      <c r="B15" s="9">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="C15" s="3">
+        <f>C14*C$1</f>
+        <v>2.8242953648100012E-2</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="F15" s="9">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12">
+      <c r="B16" s="9">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="C16" s="3">
+        <f>C15*C$1</f>
+        <v>2.5418658283290013E-2</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="F16" s="9">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12">
+      <c r="B17" s="9">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" ref="C17:C33" si="2">C16*C$1</f>
+        <v>2.2876792454961013E-2</v>
+      </c>
+      <c r="D17" s="3">
+        <f>SUM(C10:C17)</f>
+        <v>0.27240576790535109</v>
+      </c>
+      <c r="F17" s="9">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="3">
+        <f>D17/1*AVERAGE(F10:F17)</f>
+        <v>0.13620288395267555</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12">
+      <c r="B18" s="10">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="2"/>
+        <v>2.0589113209464913E-2</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="F18" s="10">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3">
+        <f t="shared" si="0"/>
+        <v>2.0589113209464913E-2</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
+      <c r="K18">
+        <v>5</v>
+      </c>
+      <c r="L18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12">
+      <c r="B19" s="10">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="C19" s="3">
+        <f t="shared" si="2"/>
+        <v>1.8530201888518422E-2</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="F19" s="10">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3">
+        <f t="shared" si="0"/>
+        <v>1.8530201888518422E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12">
+      <c r="B20" s="10">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" si="2"/>
+        <v>1.6677181699666581E-2</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="F20" s="10">
+        <v>1</v>
+      </c>
+      <c r="G20" s="3">
+        <f t="shared" si="0"/>
+        <v>1.6677181699666581E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12">
+      <c r="B21" s="10">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="C21" s="3">
+        <f t="shared" si="2"/>
+        <v>1.5009463529699923E-2</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="F21" s="10">
+        <v>1</v>
+      </c>
+      <c r="G21" s="3">
+        <f t="shared" si="0"/>
+        <v>1.5009463529699923E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12">
+      <c r="B22" s="10">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="2"/>
+        <v>1.3508517176729932E-2</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="F22" s="10">
+        <v>1</v>
+      </c>
+      <c r="G22" s="3">
+        <f t="shared" si="0"/>
+        <v>1.3508517176729932E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12">
+      <c r="B23" s="10">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="C23" s="3">
+        <f t="shared" si="2"/>
+        <v>1.215766545905694E-2</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="F23" s="10">
+        <v>1</v>
+      </c>
+      <c r="G23" s="3">
+        <f t="shared" si="0"/>
+        <v>1.215766545905694E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12">
+      <c r="B24" s="10">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0941898913151246E-2</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="F24" s="10">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12">
+      <c r="B25" s="10">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="C25" s="3">
+        <f t="shared" si="2"/>
+        <v>9.8477090218361211E-3</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="F25" s="10">
+        <v>0</v>
+      </c>
+      <c r="G25" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12">
+      <c r="B26" s="10">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="C26" s="3">
+        <f t="shared" si="2"/>
+        <v>8.8629381196525091E-3</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="F26" s="10">
+        <v>0</v>
+      </c>
+      <c r="G26" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12">
+      <c r="B27" s="10">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="C27" s="3">
+        <f t="shared" si="2"/>
+        <v>7.9766443076872591E-3</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="F27" s="10">
+        <v>0</v>
+      </c>
+      <c r="G27" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12">
+      <c r="B28" s="10">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="C28" s="3">
+        <f t="shared" si="2"/>
+        <v>7.1789798769185337E-3</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="F28" s="10">
+        <v>0</v>
+      </c>
+      <c r="G28" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12">
+      <c r="B29" s="10">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="C29" s="3">
+        <f t="shared" si="2"/>
+        <v>6.4610818892266806E-3</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="F29" s="10">
+        <v>0</v>
+      </c>
+      <c r="G29" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12">
+      <c r="B30" s="10">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="C30" s="3">
+        <f t="shared" si="2"/>
+        <v>5.8149737003040129E-3</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="F30" s="10">
+        <v>0</v>
+      </c>
+      <c r="G30" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12">
+      <c r="B31" s="10">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="C31" s="3">
+        <f t="shared" si="2"/>
+        <v>5.2334763302736113E-3</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="F31" s="10">
+        <v>0</v>
+      </c>
+      <c r="G31" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12">
+      <c r="B32" s="10">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="C32" s="3">
+        <f t="shared" si="2"/>
+        <v>4.7101286972462504E-3</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="F32" s="10">
+        <v>0</v>
+      </c>
+      <c r="G32" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8">
+      <c r="B33" s="10">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="C33" s="3">
+        <f t="shared" si="2"/>
+        <v>4.2391158275216258E-3</v>
+      </c>
+      <c r="D33" s="3">
+        <f>SUM(C18:C33)</f>
+        <v>0.16773908964695455</v>
+      </c>
+      <c r="F33" s="10">
+        <v>0</v>
+      </c>
+      <c r="G33" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H33" s="3">
+        <f>D33/1*AVERAGE(F18:F33)</f>
+        <v>6.2902158617607951E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="C36" s="3">
+        <f>SUM(C3:C33)</f>
+        <v>0.96184795755230557</v>
+      </c>
+      <c r="D36" s="3">
+        <f>SUM(D3:D33)</f>
+        <v>0.96184795755230557</v>
+      </c>
+      <c r="G36" s="3">
+        <f>SUM(G3:G33)</f>
+        <v>0.48946844687313679</v>
+      </c>
+      <c r="H36" s="3">
+        <f>SUM(H3:H33)</f>
+        <v>0.4099565925702835</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8">
+      <c r="H37" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New table to be filled in
</commit_message>
<xml_diff>
--- a/alistair/doodles.xlsx
+++ b/alistair/doodles.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="groups" sheetId="1" r:id="rId1"/>
+    <sheet name="rbp-bounds" sheetId="2" r:id="rId2"/>
+    <sheet name="geomean" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>rho</t>
   </si>
@@ -45,20 +46,64 @@
   <si>
     <t>smoothed</t>
   </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>gain</t>
+  </si>
+  <si>
+    <t>avg weight</t>
+  </si>
+  <si>
+    <t>avg gain</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Geomean</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>gavg weight</t>
+  </si>
+  <si>
+    <t>gavg gain</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
     <numFmt numFmtId="166" formatCode="0.00000000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -117,10 +162,44 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -132,8 +211,43 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="35">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -401,7 +515,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -411,7 +525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -1097,7 +1211,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="3">
-        <f>C3*C$1</f>
+        <f t="shared" ref="C4:C16" si="0">C3*C$1</f>
         <v>8.9999999999999983E-2</v>
       </c>
       <c r="D4" s="3"/>
@@ -1105,7 +1219,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="3">
-        <f t="shared" ref="G4:G33" si="0">F4*C4</f>
+        <f t="shared" ref="G4:G33" si="1">F4*C4</f>
         <v>8.9999999999999983E-2</v>
       </c>
       <c r="J4">
@@ -1120,11 +1234,11 @@
     </row>
     <row r="5" spans="2:12">
       <c r="B5" s="6">
-        <f t="shared" ref="B5:B33" si="1">B4+1</f>
+        <f t="shared" ref="B5:B33" si="2">B4+1</f>
         <v>3</v>
       </c>
       <c r="C5" s="3">
-        <f>C4*C$1</f>
+        <f t="shared" si="0"/>
         <v>8.0999999999999989E-2</v>
       </c>
       <c r="D5" s="3">
@@ -1135,7 +1249,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H5" s="3">
@@ -1145,11 +1259,11 @@
     </row>
     <row r="6" spans="2:12">
       <c r="B6" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="C6" s="3">
-        <f>C5*C$1</f>
+        <f t="shared" si="0"/>
         <v>7.2899999999999993E-2</v>
       </c>
       <c r="D6" s="3"/>
@@ -1157,7 +1271,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.2899999999999993E-2</v>
       </c>
       <c r="J6">
@@ -1172,11 +1286,11 @@
     </row>
     <row r="7" spans="2:12">
       <c r="B7" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="C7" s="3">
-        <f>C6*C$1</f>
+        <f t="shared" si="0"/>
         <v>6.5610000000000002E-2</v>
       </c>
       <c r="D7" s="3"/>
@@ -1184,17 +1298,17 @@
         <v>1</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.5610000000000002E-2</v>
       </c>
     </row>
     <row r="8" spans="2:12">
       <c r="B8" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="C8" s="3">
-        <f>C7*C$1</f>
+        <f t="shared" si="0"/>
         <v>5.9049000000000004E-2</v>
       </c>
       <c r="D8" s="3"/>
@@ -1202,17 +1316,17 @@
         <v>0</v>
       </c>
       <c r="G8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:12">
       <c r="B9" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="C9" s="3">
-        <f>C8*C$1</f>
+        <f t="shared" si="0"/>
         <v>5.3144100000000007E-2</v>
       </c>
       <c r="D9" s="3">
@@ -1223,7 +1337,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H9" s="3">
@@ -1233,11 +1347,11 @@
     </row>
     <row r="10" spans="2:12">
       <c r="B10" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="C10" s="3">
-        <f>C9*C$1</f>
+        <f t="shared" si="0"/>
         <v>4.7829690000000008E-2</v>
       </c>
       <c r="D10" s="3"/>
@@ -1245,7 +1359,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.7829690000000008E-2</v>
       </c>
       <c r="J10">
@@ -1260,11 +1374,11 @@
     </row>
     <row r="11" spans="2:12">
       <c r="B11" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="C11" s="3">
-        <f>C10*C$1</f>
+        <f t="shared" si="0"/>
         <v>4.304672100000001E-2</v>
       </c>
       <c r="D11" s="3"/>
@@ -1272,17 +1386,17 @@
         <v>1</v>
       </c>
       <c r="G11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.304672100000001E-2</v>
       </c>
     </row>
     <row r="12" spans="2:12">
       <c r="B12" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="C12" s="3">
-        <f>C11*C$1</f>
+        <f t="shared" si="0"/>
         <v>3.8742048900000013E-2</v>
       </c>
       <c r="D12" s="3"/>
@@ -1290,17 +1404,17 @@
         <v>1</v>
       </c>
       <c r="G12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.8742048900000013E-2</v>
       </c>
     </row>
     <row r="13" spans="2:12">
       <c r="B13" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="C13" s="3">
-        <f>C12*C$1</f>
+        <f t="shared" si="0"/>
         <v>3.486784401000001E-2</v>
       </c>
       <c r="D13" s="3"/>
@@ -1308,17 +1422,17 @@
         <v>1</v>
       </c>
       <c r="G13" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.486784401000001E-2</v>
       </c>
     </row>
     <row r="14" spans="2:12">
       <c r="B14" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="C14" s="3">
-        <f>C13*C$1</f>
+        <f t="shared" si="0"/>
         <v>3.1381059609000013E-2</v>
       </c>
       <c r="D14" s="3"/>
@@ -1326,17 +1440,17 @@
         <v>0</v>
       </c>
       <c r="G14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:12">
       <c r="B15" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="C15" s="3">
-        <f>C14*C$1</f>
+        <f t="shared" si="0"/>
         <v>2.8242953648100012E-2</v>
       </c>
       <c r="D15" s="3"/>
@@ -1344,17 +1458,17 @@
         <v>0</v>
       </c>
       <c r="G15" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:12">
       <c r="B16" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="C16" s="3">
-        <f>C15*C$1</f>
+        <f t="shared" si="0"/>
         <v>2.5418658283290013E-2</v>
       </c>
       <c r="D16" s="3"/>
@@ -1362,17 +1476,17 @@
         <v>0</v>
       </c>
       <c r="G16" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:12">
       <c r="B17" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="C17" s="3">
-        <f t="shared" ref="C17:C33" si="2">C16*C$1</f>
+        <f t="shared" ref="C17:C33" si="3">C16*C$1</f>
         <v>2.2876792454961013E-2</v>
       </c>
       <c r="D17" s="3">
@@ -1383,7 +1497,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H17" s="3">
@@ -1393,11 +1507,11 @@
     </row>
     <row r="18" spans="2:12">
       <c r="B18" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="C18" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.0589113209464913E-2</v>
       </c>
       <c r="D18" s="3"/>
@@ -1405,7 +1519,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.0589113209464913E-2</v>
       </c>
       <c r="J18">
@@ -1420,11 +1534,11 @@
     </row>
     <row r="19" spans="2:12">
       <c r="B19" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="C19" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8530201888518422E-2</v>
       </c>
       <c r="D19" s="3"/>
@@ -1432,17 +1546,17 @@
         <v>1</v>
       </c>
       <c r="G19" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.8530201888518422E-2</v>
       </c>
     </row>
     <row r="20" spans="2:12">
       <c r="B20" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="C20" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.6677181699666581E-2</v>
       </c>
       <c r="D20" s="3"/>
@@ -1450,17 +1564,17 @@
         <v>1</v>
       </c>
       <c r="G20" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.6677181699666581E-2</v>
       </c>
     </row>
     <row r="21" spans="2:12">
       <c r="B21" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="C21" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.5009463529699923E-2</v>
       </c>
       <c r="D21" s="3"/>
@@ -1468,17 +1582,17 @@
         <v>1</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5009463529699923E-2</v>
       </c>
     </row>
     <row r="22" spans="2:12">
       <c r="B22" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="C22" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3508517176729932E-2</v>
       </c>
       <c r="D22" s="3"/>
@@ -1486,17 +1600,17 @@
         <v>1</v>
       </c>
       <c r="G22" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3508517176729932E-2</v>
       </c>
     </row>
     <row r="23" spans="2:12">
       <c r="B23" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="C23" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.215766545905694E-2</v>
       </c>
       <c r="D23" s="3"/>
@@ -1504,17 +1618,17 @@
         <v>1</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.215766545905694E-2</v>
       </c>
     </row>
     <row r="24" spans="2:12">
       <c r="B24" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="C24" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0941898913151246E-2</v>
       </c>
       <c r="D24" s="3"/>
@@ -1522,17 +1636,17 @@
         <v>0</v>
       </c>
       <c r="G24" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:12">
       <c r="B25" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="C25" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.8477090218361211E-3</v>
       </c>
       <c r="D25" s="3"/>
@@ -1540,17 +1654,17 @@
         <v>0</v>
       </c>
       <c r="G25" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:12">
       <c r="B26" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="C26" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.8629381196525091E-3</v>
       </c>
       <c r="D26" s="3"/>
@@ -1558,17 +1672,17 @@
         <v>0</v>
       </c>
       <c r="G26" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:12">
       <c r="B27" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="C27" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.9766443076872591E-3</v>
       </c>
       <c r="D27" s="3"/>
@@ -1576,17 +1690,17 @@
         <v>0</v>
       </c>
       <c r="G27" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:12">
       <c r="B28" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="C28" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.1789798769185337E-3</v>
       </c>
       <c r="D28" s="3"/>
@@ -1594,17 +1708,17 @@
         <v>0</v>
       </c>
       <c r="G28" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:12">
       <c r="B29" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="C29" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.4610818892266806E-3</v>
       </c>
       <c r="D29" s="3"/>
@@ -1612,17 +1726,17 @@
         <v>0</v>
       </c>
       <c r="G29" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:12">
       <c r="B30" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="C30" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.8149737003040129E-3</v>
       </c>
       <c r="D30" s="3"/>
@@ -1630,17 +1744,17 @@
         <v>0</v>
       </c>
       <c r="G30" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:12">
       <c r="B31" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="C31" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.2334763302736113E-3</v>
       </c>
       <c r="D31" s="3"/>
@@ -1648,17 +1762,17 @@
         <v>0</v>
       </c>
       <c r="G31" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:12">
       <c r="B32" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="C32" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.7101286972462504E-3</v>
       </c>
       <c r="D32" s="3"/>
@@ -1666,17 +1780,17 @@
         <v>0</v>
       </c>
       <c r="G32" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:8">
       <c r="B33" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="C33" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.2391158275216258E-3</v>
       </c>
       <c r="D33" s="3">
@@ -1687,7 +1801,7 @@
         <v>0</v>
       </c>
       <c r="G33" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H33" s="3">
@@ -1724,4 +1838,549 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:Q20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="6" max="6" width="3.33203125" customWidth="1"/>
+    <col min="11" max="11" width="3.33203125" customWidth="1"/>
+    <col min="16" max="16" width="2.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:17">
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17">
+      <c r="D3" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11">
+        <f>E3*D3</f>
+        <v>0.1</v>
+      </c>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11">
+        <f>AVERAGE(D$3:D$7)</f>
+        <v>0.26339999999999997</v>
+      </c>
+      <c r="J3" s="11">
+        <f>E3</f>
+        <v>0.2</v>
+      </c>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11">
+        <f>J3*I3</f>
+        <v>5.2679999999999998E-2</v>
+      </c>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11">
+        <f>D3</f>
+        <v>0.5</v>
+      </c>
+      <c r="O3" s="11">
+        <f>AVERAGE(E$3:E$7)</f>
+        <v>0.2</v>
+      </c>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11">
+        <f>O3*N3</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17">
+      <c r="D4" s="11">
+        <v>0.217</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11">
+        <f>E4*D4</f>
+        <v>6.5099999999999991E-2</v>
+      </c>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11">
+        <f>AVERAGE(D$3:D$7)</f>
+        <v>0.26339999999999997</v>
+      </c>
+      <c r="J4" s="11">
+        <f>E4</f>
+        <v>0.3</v>
+      </c>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11">
+        <f>J4*I4</f>
+        <v>7.9019999999999993E-2</v>
+      </c>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11">
+        <f>D4</f>
+        <v>0.217</v>
+      </c>
+      <c r="O4" s="11">
+        <f>AVERAGE(E$3:E$7)</f>
+        <v>0.2</v>
+      </c>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11">
+        <f>O4*N4</f>
+        <v>4.3400000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17">
+      <c r="D5" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="E5" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11">
+        <f>E5*D5</f>
+        <v>0.06</v>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11">
+        <f>AVERAGE(D$3:D$7)</f>
+        <v>0.26339999999999997</v>
+      </c>
+      <c r="J5" s="11">
+        <f>E5</f>
+        <v>0.2</v>
+      </c>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11">
+        <f>J5*I5</f>
+        <v>5.2679999999999998E-2</v>
+      </c>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11">
+        <f>D5</f>
+        <v>0.3</v>
+      </c>
+      <c r="O5" s="11">
+        <f>AVERAGE(E$3:E$7)</f>
+        <v>0.2</v>
+      </c>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11">
+        <f>O5*N5</f>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17">
+      <c r="D6" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="E6" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11">
+        <f>E6*D6</f>
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11">
+        <f>AVERAGE(D$3:D$7)</f>
+        <v>0.26339999999999997</v>
+      </c>
+      <c r="J6" s="11">
+        <f>E6</f>
+        <v>0.1</v>
+      </c>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11">
+        <f>J6*I6</f>
+        <v>2.6339999999999999E-2</v>
+      </c>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11">
+        <f>D6</f>
+        <v>0.2</v>
+      </c>
+      <c r="O6" s="11">
+        <f>AVERAGE(E$3:E$7)</f>
+        <v>0.2</v>
+      </c>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11">
+        <f>O6*N6</f>
+        <v>4.0000000000000008E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17">
+      <c r="D7" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="E7" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11">
+        <f>E7*D7</f>
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11">
+        <f>AVERAGE(D$3:D$7)</f>
+        <v>0.26339999999999997</v>
+      </c>
+      <c r="J7" s="11">
+        <f>E7</f>
+        <v>0.2</v>
+      </c>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11">
+        <f>J7*I7</f>
+        <v>5.2679999999999998E-2</v>
+      </c>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11">
+        <f>D7</f>
+        <v>0.1</v>
+      </c>
+      <c r="O7" s="11">
+        <f>AVERAGE(E$3:E$7)</f>
+        <v>0.2</v>
+      </c>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11">
+        <f>O7*N7</f>
+        <v>2.0000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17">
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+    </row>
+    <row r="9" spans="2:17">
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11">
+        <f>SUM(G3:G7)</f>
+        <v>0.2651</v>
+      </c>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11">
+        <f>SUM(L3:L7)</f>
+        <v>0.26339999999999997</v>
+      </c>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11">
+        <f>SUM(Q3:Q7)</f>
+        <v>0.26340000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" t="s">
+        <v>8</v>
+      </c>
+      <c r="L12" t="s">
+        <v>13</v>
+      </c>
+      <c r="N12" t="s">
+        <v>7</v>
+      </c>
+      <c r="O12" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17">
+      <c r="D14" s="11">
+        <f>D3</f>
+        <v>0.5</v>
+      </c>
+      <c r="E14" s="11">
+        <f t="shared" ref="E14:E18" si="0">E3</f>
+        <v>0.2</v>
+      </c>
+      <c r="G14" s="11">
+        <f>E14*D14</f>
+        <v>0.1</v>
+      </c>
+      <c r="I14">
+        <f>POWER(PRODUCT(D$3:D$7),1/5)</f>
+        <v>0.23052402704957323</v>
+      </c>
+      <c r="J14" s="11">
+        <f>E14</f>
+        <v>0.2</v>
+      </c>
+      <c r="L14" s="11">
+        <f>J14*I14</f>
+        <v>4.610480540991465E-2</v>
+      </c>
+      <c r="N14" s="11">
+        <f>D14</f>
+        <v>0.5</v>
+      </c>
+      <c r="O14">
+        <f>POWER(PRODUCT(E$3:E$7),1/5)</f>
+        <v>0.18881750225898036</v>
+      </c>
+      <c r="Q14" s="11">
+        <f>O14*N14</f>
+        <v>9.4408751129490182E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17">
+      <c r="D15" s="11">
+        <f t="shared" ref="D15:E15" si="1">D4</f>
+        <v>0.217</v>
+      </c>
+      <c r="E15" s="11">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="G15" s="11">
+        <f>E15*D15</f>
+        <v>6.5099999999999991E-2</v>
+      </c>
+      <c r="I15">
+        <f>POWER(PRODUCT(D$3:D$7),1/5)</f>
+        <v>0.23052402704957323</v>
+      </c>
+      <c r="J15" s="11">
+        <f>E15</f>
+        <v>0.3</v>
+      </c>
+      <c r="L15" s="11">
+        <f>J15*I15</f>
+        <v>6.9157208114871971E-2</v>
+      </c>
+      <c r="N15" s="11">
+        <f>D15</f>
+        <v>0.217</v>
+      </c>
+      <c r="O15">
+        <f>POWER(PRODUCT(E$3:E$7),1/5)</f>
+        <v>0.18881750225898036</v>
+      </c>
+      <c r="Q15" s="11">
+        <f>O15*N15</f>
+        <v>4.0973397990198737E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17">
+      <c r="D16" s="11">
+        <f t="shared" ref="D16:E16" si="2">D5</f>
+        <v>0.3</v>
+      </c>
+      <c r="E16" s="11">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="G16" s="11">
+        <f>E16*D16</f>
+        <v>0.06</v>
+      </c>
+      <c r="I16">
+        <f>POWER(PRODUCT(D$3:D$7),1/5)</f>
+        <v>0.23052402704957323</v>
+      </c>
+      <c r="J16" s="11">
+        <f>E16</f>
+        <v>0.2</v>
+      </c>
+      <c r="L16" s="11">
+        <f>J16*I16</f>
+        <v>4.610480540991465E-2</v>
+      </c>
+      <c r="N16" s="11">
+        <f>D16</f>
+        <v>0.3</v>
+      </c>
+      <c r="O16">
+        <f>POWER(PRODUCT(E$3:E$7),1/5)</f>
+        <v>0.18881750225898036</v>
+      </c>
+      <c r="Q16" s="11">
+        <f>O16*N16</f>
+        <v>5.6645250677694103E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="4:17">
+      <c r="D17" s="11">
+        <f t="shared" ref="D17:E17" si="3">D6</f>
+        <v>0.2</v>
+      </c>
+      <c r="E17" s="11">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="G17" s="11">
+        <f>E17*D17</f>
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="I17">
+        <f>POWER(PRODUCT(D$3:D$7),1/5)</f>
+        <v>0.23052402704957323</v>
+      </c>
+      <c r="J17" s="11">
+        <f>E17</f>
+        <v>0.1</v>
+      </c>
+      <c r="L17" s="11">
+        <f>J17*I17</f>
+        <v>2.3052402704957325E-2</v>
+      </c>
+      <c r="N17" s="11">
+        <f>D17</f>
+        <v>0.2</v>
+      </c>
+      <c r="O17">
+        <f>POWER(PRODUCT(E$3:E$7),1/5)</f>
+        <v>0.18881750225898036</v>
+      </c>
+      <c r="Q17" s="11">
+        <f>O17*N17</f>
+        <v>3.7763500451796078E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="4:17">
+      <c r="D18" s="11">
+        <f t="shared" ref="D18:E18" si="4">D7</f>
+        <v>0.1</v>
+      </c>
+      <c r="E18" s="11">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="G18" s="11">
+        <f>E18*D18</f>
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="I18">
+        <f>POWER(PRODUCT(D$3:D$7),1/5)</f>
+        <v>0.23052402704957323</v>
+      </c>
+      <c r="J18" s="11">
+        <f>E18</f>
+        <v>0.2</v>
+      </c>
+      <c r="L18" s="11">
+        <f>J18*I18</f>
+        <v>4.610480540991465E-2</v>
+      </c>
+      <c r="N18" s="11">
+        <f>D18</f>
+        <v>0.1</v>
+      </c>
+      <c r="O18">
+        <f>POWER(PRODUCT(E$3:E$7),1/5)</f>
+        <v>0.18881750225898036</v>
+      </c>
+      <c r="Q18" s="11">
+        <f>O18*N18</f>
+        <v>1.8881750225898039E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="4:17">
+      <c r="G19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="Q19" s="11"/>
+    </row>
+    <row r="20" spans="4:17">
+      <c r="G20" s="11">
+        <f>SUM(G14:G18)</f>
+        <v>0.2651</v>
+      </c>
+      <c r="L20" s="11">
+        <f>SUM(L14:L18)</f>
+        <v>0.23052402704957325</v>
+      </c>
+      <c r="Q20" s="11">
+        <f>SUM(Q14:Q18)</f>
+        <v>0.24867265047507714</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>